<commit_message>
fix: add additional manual SNPs from: Acute pancreatitis risk in multifactorial chylomicronemia syndrome depends on the molecular cause of severe hypertriglyceridemia PMID: 38448342
</commit_message>
<xml_diff>
--- a/data/snp/manual/manual.xlsx
+++ b/data/snp/manual/manual.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A44DAA8-E9AF-436A-87A8-A2631E236ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFAB63A-2673-4DFA-A9C1-51643FA0A7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
   <si>
     <t>rs_id</t>
   </si>
@@ -147,6 +147,60 @@
   </si>
   <si>
     <t>C marks the ε4 allele, which is associated with higher LDL cholesterol; Futema et al. 2015 (LDL-C-Score (PMID: 25414277)</t>
+  </si>
+  <si>
+    <t>rs4846914</t>
+  </si>
+  <si>
+    <t>rs17145738</t>
+  </si>
+  <si>
+    <t>rs1495741</t>
+  </si>
+  <si>
+    <t>rs12678919</t>
+  </si>
+  <si>
+    <t>rs10761731</t>
+  </si>
+  <si>
+    <t>rs2412710</t>
+  </si>
+  <si>
+    <t>rs2929282</t>
+  </si>
+  <si>
+    <t>rs10401969</t>
+  </si>
+  <si>
+    <t>rs6065906</t>
+  </si>
+  <si>
+    <t>Guay et al. 2024 (Acute pancreatitis risk in multifactorial chylomicronemia syndrome depends on the molecular cause of severe hypertriglyceridemia; PMID: 38448342)</t>
+  </si>
+  <si>
+    <t>GALNT2</t>
+  </si>
+  <si>
+    <t>MLXIPL</t>
+  </si>
+  <si>
+    <t>NAT2</t>
+  </si>
+  <si>
+    <t>JMJD1C</t>
+  </si>
+  <si>
+    <t>CAPN3</t>
+  </si>
+  <si>
+    <t>FRMD5</t>
+  </si>
+  <si>
+    <t>CSPG3, CILP2, PBX4</t>
+  </si>
+  <si>
+    <t>PLTP</t>
   </si>
 </sst>
 </file>
@@ -701,7 +755,27 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1017,7 +1091,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1027,8 +1101,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="135.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="182.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -1240,10 +1314,110 @@
         <v>40</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add DPYD variant
</commit_message>
<xml_diff>
--- a/data/snp/manual/manual.xlsx
+++ b/data/snp/manual/manual.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFAB63A-2673-4DFA-A9C1-51643FA0A7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4D1F1B-4B09-4D88-8E79-7A81D9AFBE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>rs_id</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t>PLTP</t>
+  </si>
+  <si>
+    <t>rs75017182</t>
+  </si>
+  <si>
+    <t>DPYD</t>
+  </si>
+  <si>
+    <t>Haplotype B3: c.1236G&gt;A; c.1129-5923C&gt;G - Compound variant</t>
   </si>
 </sst>
 </file>
@@ -755,17 +764,7 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1091,7 +1090,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1413,11 +1412,22 @@
         <v>52</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add OC and BC SNPS for prostate cacner PRS manually from publications that are not in PGS Juliette Coignard et al. 2021: https://www.nature.com/articles/s41467-020-20496-3 Lee et al. 2022: https://jmg.bmj.com/content/59/7/632.long#DC1
</commit_message>
<xml_diff>
--- a/data/snp/manual/manual.xlsx
+++ b/data/snp/manual/manual.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4D1F1B-4B09-4D88-8E79-7A81D9AFBE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9C7595-50AC-4815-9E3D-FAEAB470ACBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual_snps" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
   <si>
     <t>rs_id</t>
   </si>
@@ -210,6 +210,144 @@
   </si>
   <si>
     <t>Haplotype B3: c.1236G&gt;A; c.1129-5923C&gt;G - Compound variant</t>
+  </si>
+  <si>
+    <t>rs58722170</t>
+  </si>
+  <si>
+    <t>rs711830</t>
+  </si>
+  <si>
+    <t>rs62274041</t>
+  </si>
+  <si>
+    <t>rs10069690</t>
+  </si>
+  <si>
+    <t>rs78724141</t>
+  </si>
+  <si>
+    <t>rs10088218</t>
+  </si>
+  <si>
+    <t>rs7032221</t>
+  </si>
+  <si>
+    <t>rs635634</t>
+  </si>
+  <si>
+    <t>rs1802669</t>
+  </si>
+  <si>
+    <t>rs7135337</t>
+  </si>
+  <si>
+    <t>rs11651755</t>
+  </si>
+  <si>
+    <t>rs1105569</t>
+  </si>
+  <si>
+    <t>rs7207826</t>
+  </si>
+  <si>
+    <t>rs61494113</t>
+  </si>
+  <si>
+    <t>rs9625477</t>
+  </si>
+  <si>
+    <t>ovarian cancer (Comprehensive epithelial tubo-ovarian cancer risk prediction model incorporating genetic and epidemiological risk factors; PMID: 34844974; Table S5)</t>
+  </si>
+  <si>
+    <t>rs60882887</t>
+  </si>
+  <si>
+    <t>rs5820435</t>
+  </si>
+  <si>
+    <t>rs7222250</t>
+  </si>
+  <si>
+    <t>rs9901834</t>
+  </si>
+  <si>
+    <t>rs58117746</t>
+  </si>
+  <si>
+    <t>rs2239711</t>
+  </si>
+  <si>
+    <t>rs10708222</t>
+  </si>
+  <si>
+    <t>rs41283425</t>
+  </si>
+  <si>
+    <t>rs56291217</t>
+  </si>
+  <si>
+    <t>rs111637825</t>
+  </si>
+  <si>
+    <t>breast cancer (A case-only study to identify genetic modifiers of breast cancer risk for BRCA1/BRCA2 mutation carriers; Table 5; PMID: 33597508)</t>
+  </si>
+  <si>
+    <t>breast cancer (A case-only study to identify genetic modifiers of breast cancer risk for BRCA1/BRCA2 mutation carriers; Table 6; PMID: 33597508)</t>
+  </si>
+  <si>
+    <t>rs12470785</t>
+  </si>
+  <si>
+    <t>rs79183898</t>
+  </si>
+  <si>
+    <t>rs71434801</t>
+  </si>
+  <si>
+    <t>rs77197167</t>
+  </si>
+  <si>
+    <t>rs114300732</t>
+  </si>
+  <si>
+    <t>13:32231513:CAA:C</t>
+  </si>
+  <si>
+    <t>rs1623189</t>
+  </si>
+  <si>
+    <t>rs736596</t>
+  </si>
+  <si>
+    <t>rs77889880</t>
+  </si>
+  <si>
+    <t>rs67776313</t>
+  </si>
+  <si>
+    <t>rs71196514</t>
+  </si>
+  <si>
+    <t>rs2555605</t>
+  </si>
+  <si>
+    <t>rs74796280</t>
+  </si>
+  <si>
+    <t>rs4943263</t>
+  </si>
+  <si>
+    <t>rs2202781</t>
+  </si>
+  <si>
+    <t>rs55675572</t>
+  </si>
+  <si>
+    <t>rs17755120</t>
+  </si>
+  <si>
+    <t>rs1198832427</t>
   </si>
 </sst>
 </file>
@@ -714,10 +852,11 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1090,11 +1229,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1423,9 +1562,348 @@
         <v>63</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C74" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A1:A60 A62:A1048576 B61">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat: update report after recalculation
</commit_message>
<xml_diff>
--- a/data/snp/manual/manual.xlsx
+++ b/data/snp/manual/manual.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9C7595-50AC-4815-9E3D-FAEAB470ACBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA7CED5-F4DE-4B49-836C-1043A8B22842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="110">
   <si>
     <t>rs_id</t>
   </si>
@@ -311,9 +311,6 @@
     <t>rs114300732</t>
   </si>
   <si>
-    <t>13:32231513:CAA:C</t>
-  </si>
-  <si>
     <t>rs1623189</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>rs1198832427</t>
+  </si>
+  <si>
+    <t>breast cancer (A case-only study to identify genetic modifiers of breast cancer risk for BRCA1/BRCA2 mutation carriers; Table 6; PMID: 33597508; described as hg19 13:32231513:CAA:C is 13-31657376-C-CAA in g38)</t>
   </si>
 </sst>
 </file>
@@ -852,11 +852,10 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1232,8 +1231,8 @@
   <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1804,18 +1803,15 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>91</v>
@@ -1823,7 +1819,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>91</v>
@@ -1831,7 +1827,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>91</v>
@@ -1839,7 +1835,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>91</v>
@@ -1847,7 +1843,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>91</v>
@@ -1855,7 +1851,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>91</v>
@@ -1863,7 +1859,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>91</v>
@@ -1871,7 +1867,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>91</v>
@@ -1879,7 +1875,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>91</v>
@@ -1887,7 +1883,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>91</v>
@@ -1895,7 +1891,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>91</v>

</xml_diff>